<commit_message>
abc styler in buying documents
</commit_message>
<xml_diff>
--- a/application/views/rpt/DocumentOut.xlsx
+++ b/application/views/rpt/DocumentOut.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4464" yWindow="0" windowWidth="17436" windowHeight="10476"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="17436" windowHeight="10476"/>
   </bookViews>
   <sheets>
     <sheet name="Экспорт" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Клиент:{$v-&gt;head-&gt;label} Документ №{$v-&gt;head-&gt;doc_num} от {$v-&gt;head-&gt;doc_date}</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>{$v-&gt;rows[]-&gt;product_sum}</t>
+  </si>
+  <si>
+    <t>Класс ABC</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;analyse_class}</t>
   </si>
 </sst>
 </file>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -515,10 +521,11 @@
     <col min="5" max="6" width="7" style="3" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="12" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="4"/>
+    <col min="9" max="9" width="12.44140625" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -530,7 +537,7 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -542,7 +549,7 @@
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -567,8 +574,11 @@
       <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="I3" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
@@ -592,6 +602,9 @@
       </c>
       <c r="H4" s="11" t="s">
         <v>17</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>